<commit_message>
Basic report layout with some graphs
</commit_message>
<xml_diff>
--- a/Game of Life Processing Times.xlsx
+++ b/Game of Life Processing Times.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jackb\Uni\GOL\game-of-life\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jackb\Documents\game-of-life\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E2CBF1C-1A0E-4D3E-A339-4DB0DBBCE0BB}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E724617D-3D11-481B-9401-C4F9CFF9815F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24720" windowHeight="12216" xr2:uid="{E68FA09E-A4D2-4ABB-831A-49156287513F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24720" windowHeight="12210" xr2:uid="{E68FA09E-A4D2-4ABB-831A-49156287513F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="40">
   <si>
     <t>average round time</t>
   </si>
@@ -89,9 +90,6 @@
     <t>All workers on tile[i%2] - distributor on tile[0]</t>
   </si>
   <si>
-    <t>LESS NEIGHBOUGH CHECKS</t>
-  </si>
-  <si>
     <t>SKIP DEAD AREAS</t>
   </si>
   <si>
@@ -126,13 +124,40 @@
   </si>
   <si>
     <t>Speedup (from before dead skipping)</t>
+  </si>
+  <si>
+    <t>Board Size</t>
+  </si>
+  <si>
+    <t>8 Worker Bit Packed</t>
+  </si>
+  <si>
+    <t>8 Worker Less Checks</t>
+  </si>
+  <si>
+    <t>8 Worker Skip Dead</t>
+  </si>
+  <si>
+    <t>4 Worker Skip Dead</t>
+  </si>
+  <si>
+    <t>4 Worker Skip Dead + Streaming</t>
+  </si>
+  <si>
+    <t>Rounds per Second</t>
+  </si>
+  <si>
+    <t>Speedup from Original (%)</t>
+  </si>
+  <si>
+    <t>LESS NEIGHBOUR CHECKS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -155,16 +180,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -172,18 +217,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -195,7 +255,75 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="10">
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="13" formatCode="0%"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -237,7 +365,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{442B4B30-4FC1-4097-B3F7-C0EC155F6426}" name="Table12" displayName="Table12" ref="I10:I18" totalsRowShown="0">
   <autoFilter ref="I10:I18" xr:uid="{58FBDD7A-3B08-4690-BCA2-2A1E023DC340}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{130C92A1-0FAE-46C4-AFB8-E6148B1A2AE3}" name="Speedup" dataDxfId="0">
+    <tableColumn id="1" xr3:uid="{130C92A1-0FAE-46C4-AFB8-E6148B1A2AE3}" name="Speedup" dataDxfId="6">
       <calculatedColumnFormula>Table2[[#This Row],[100 rounds time]]/Table3[[#This Row],[100 rounds time]] - 1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -278,6 +406,54 @@
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{2D5E1AE7-75EF-4CC0-B131-8064CA253326}" name="Table4" displayName="Table4" ref="A51:F58" totalsRowShown="0">
+  <autoFilter ref="A51:F58" xr:uid="{DA563CAA-AB3B-464C-9D40-321E7802B9E9}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{B10DB1CE-67BC-4CA7-803C-FB3EF49BE94B}" name="Board Size"/>
+    <tableColumn id="2" xr3:uid="{DE4FD451-F950-44A5-9BA2-F72A6D1D9138}" name="8 Worker Bit Packed" dataDxfId="5" dataCellStyle="Percent">
+      <calculatedColumnFormula>(100/F11)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{A9939D9E-C884-4647-B829-11649DFC879D}" name="8 Worker Less Checks">
+      <calculatedColumnFormula>100/B22</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{2A1BBDFF-A014-4210-88E9-E3B7770EEC17}" name="8 Worker Skip Dead"/>
+    <tableColumn id="5" xr3:uid="{175F6779-EA0A-4DFE-8053-B8232379AAAB}" name="4 Worker Skip Dead">
+      <calculatedColumnFormula>100/B42</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{BEC47713-7D14-439E-9F88-C76B2539BB24}" name="4 Worker Skip Dead + Streaming">
+      <calculatedColumnFormula>100/F42</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{92339985-C53F-45DE-8BF4-7B0B6B157643}" name="Table49" displayName="Table49" ref="A61:F68" totalsRowShown="0">
+  <autoFilter ref="A61:F68" xr:uid="{D6884FC4-5E41-4485-A15D-A67D31681683}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{57A574EF-9193-42B3-9868-B6B09E8E3996}" name="Board Size"/>
+    <tableColumn id="2" xr3:uid="{A14823A9-1A21-4677-9256-42198EB6F238}" name="8 Worker Bit Packed" dataDxfId="4" dataCellStyle="Percent">
+      <calculatedColumnFormula>B52/B52 - 1</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{FEEF9E3D-472E-482F-9D6F-552352A02E66}" name="8 Worker Less Checks" dataDxfId="3" dataCellStyle="Percent">
+      <calculatedColumnFormula>C52/B52 - 1</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{06266E42-2CD8-41DE-87C2-CDD4CC8CCCB4}" name="8 Worker Skip Dead" dataDxfId="2" dataCellStyle="Percent">
+      <calculatedColumnFormula>D52/B52  - 1</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{D1BBADC8-4606-4F1F-818A-EB968FAC3969}" name="4 Worker Skip Dead" dataDxfId="1" dataCellStyle="Percent">
+      <calculatedColumnFormula>E52/B52  - 1</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{B228D484-7E2D-45F4-BA6C-B91B74EFFDAD}" name="4 Worker Skip Dead + Streaming" dataDxfId="0" dataCellStyle="Percent">
+      <calculatedColumnFormula>F52/B52  - 1</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -351,7 +527,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{A323AE7C-2B2A-4858-A4A7-0FC31B36838D}" name="Table9" displayName="Table9" ref="I31:I38" totalsRowShown="0">
   <autoFilter ref="I31:I38" xr:uid="{3C9D786D-D041-4939-8FFC-7A8AF5FAD749}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{837FD844-21A5-451B-BFB5-F33BFE6CF349}" name="Speedup" dataDxfId="3">
+    <tableColumn id="1" xr3:uid="{837FD844-21A5-451B-BFB5-F33BFE6CF349}" name="Speedup" dataDxfId="9">
       <calculatedColumnFormula>Table367[[#This Row],[100 rounds time]]-Table3678[[#This Row],[100 rounds time]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -365,7 +541,7 @@
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{EA40BF43-2D31-4701-A06F-06C4AF9FD639}" name="4 WORKERS"/>
     <tableColumn id="2" xr3:uid="{2903E8B1-0E02-48A9-A3FF-D20F0D0AF6EE}" name="100 rounds time"/>
-    <tableColumn id="3" xr3:uid="{08B59550-F6C3-44E7-9297-A8A316B6288D}" name="average round time" dataDxfId="2">
+    <tableColumn id="3" xr3:uid="{08B59550-F6C3-44E7-9297-A8A316B6288D}" name="average round time" dataDxfId="8">
       <calculatedColumnFormula>Table10[[#This Row],[100 rounds time]]/100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -379,7 +555,7 @@
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{3AFCD051-07E8-4D50-B675-0A492DEF6BB5}" name="4 WORKERS"/>
     <tableColumn id="2" xr3:uid="{4552D035-3B3A-411A-BE1D-8F2454F1BA37}" name="100 rounds time"/>
-    <tableColumn id="3" xr3:uid="{AA99BE11-F653-4AED-9F3E-F21320BB0E43}" name="average round time" dataDxfId="1">
+    <tableColumn id="3" xr3:uid="{AA99BE11-F653-4AED-9F3E-F21320BB0E43}" name="average round time" dataDxfId="7">
       <calculatedColumnFormula>Table1012[[#This Row],[100 rounds time]]/100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -684,25 +860,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7C0B61C-51FD-49C9-903F-698AAA3C829E}">
-  <dimension ref="A1:K48"/>
+  <dimension ref="A1:K68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="J58" sqref="J58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.109375" customWidth="1"/>
-    <col min="2" max="2" width="20.33203125" customWidth="1"/>
-    <col min="3" max="3" width="20.44140625" customWidth="1"/>
-    <col min="5" max="5" width="20.21875" customWidth="1"/>
-    <col min="6" max="6" width="20.33203125" customWidth="1"/>
-    <col min="7" max="7" width="20.44140625" customWidth="1"/>
-    <col min="9" max="9" width="21.6640625" customWidth="1"/>
-    <col min="11" max="11" width="22.6640625" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" customWidth="1"/>
+    <col min="5" max="5" width="23.85546875" customWidth="1"/>
+    <col min="6" max="6" width="34.140625" customWidth="1"/>
+    <col min="7" max="7" width="20.42578125" customWidth="1"/>
+    <col min="9" max="9" width="21.7109375" customWidth="1"/>
+    <col min="11" max="11" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -710,7 +887,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -721,7 +898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -733,7 +910,7 @@
         <v>1.12078E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -745,7 +922,7 @@
         <v>1.559286E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -757,7 +934,7 @@
         <v>6.103455E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -769,7 +946,7 @@
         <v>0.23974155</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -780,21 +957,21 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="4"/>
-      <c r="E9" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B9" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="8"/>
+      <c r="E9" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -814,10 +991,10 @@
         <v>0</v>
       </c>
       <c r="I10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -843,7 +1020,7 @@
         <v>0.24824760198165907</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -869,7 +1046,7 @@
         <v>0.25938463026381164</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -895,7 +1072,7 @@
         <v>0.24527921645106709</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -921,7 +1098,7 @@
         <v>0.24662013569531327</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -947,7 +1124,7 @@
         <v>0.24740072258319556</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -973,7 +1150,7 @@
         <v>0.24722966021208537</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -999,7 +1176,7 @@
         <v>0.24729921755480144</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -1019,15 +1196,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -1038,10 +1215,10 @@
         <v>0</v>
       </c>
       <c r="E21" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>1</v>
       </c>
@@ -1057,7 +1234,7 @@
         <v>0.15206897598591329</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>2</v>
       </c>
@@ -1073,7 +1250,7 @@
         <v>0.13083330681980865</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>3</v>
       </c>
@@ -1089,7 +1266,7 @@
         <v>0.13073262135994401</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>4</v>
       </c>
@@ -1105,23 +1282,23 @@
         <v>0.14805452306279565</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>5</v>
       </c>
       <c r="B26">
-        <v>67.297393999999997</v>
+        <v>62.707306000000003</v>
       </c>
       <c r="C26">
         <f>Table36[[#This Row],[100 rounds time]]/100</f>
-        <v>0.67297393999999999</v>
+        <v>0.62707306000000007</v>
       </c>
       <c r="E26" s="3">
         <f>F15/Table36[[#This Row],[100 rounds time]] - 1</f>
-        <v>7.9502276120825721E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+        <v>0.15852034849017427</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>11</v>
       </c>
@@ -1137,7 +1314,7 @@
         <v>7.8944700077026475E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>13</v>
       </c>
@@ -1153,21 +1330,21 @@
         <v>5.079350311388775E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="E30" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G30" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E30" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>12</v>
       </c>
@@ -1187,13 +1364,13 @@
         <v>0</v>
       </c>
       <c r="I31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K31" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>1</v>
       </c>
@@ -1218,7 +1395,7 @@
         <v>0.44367987377279117</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>2</v>
       </c>
@@ -1248,7 +1425,7 @@
         <v>0.4648666834644386</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>3</v>
       </c>
@@ -1278,7 +1455,7 @@
         <v>0.87735892896144407</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>4</v>
       </c>
@@ -1308,9 +1485,9 @@
         <v>0.60895392685668615</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B36">
         <v>38.607723</v>
@@ -1320,7 +1497,7 @@
         <v>0.38607722999999999</v>
       </c>
       <c r="E36" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F36">
         <v>38.147499000000003</v>
@@ -1335,10 +1512,10 @@
       </c>
       <c r="K36" s="3">
         <f>B26/Table367[[#This Row],[100 rounds time]] - 1</f>
-        <v>0.7431070462249223</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+        <v>0.62421663665583194</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>11</v>
       </c>
@@ -1368,39 +1545,45 @@
         <v>2.3612055101885909E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>13</v>
       </c>
+      <c r="B38">
+        <v>436.016052</v>
+      </c>
       <c r="C38">
         <f>Table367[[#This Row],[100 rounds time]]/100</f>
-        <v>0</v>
+        <v>4.36016052</v>
       </c>
       <c r="E38" t="s">
         <v>13</v>
       </c>
+      <c r="F38">
+        <v>422.51650999999998</v>
+      </c>
       <c r="G38">
         <f>Table3678[[#This Row],[100 rounds time]]/100</f>
-        <v>0</v>
-      </c>
-      <c r="I38" s="3" t="e">
+        <v>4.2251650999999999</v>
+      </c>
+      <c r="I38" s="3">
         <f>Table367[[#This Row],[100 rounds time]]/Table3678[[#This Row],[100 rounds time]] - 1</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K38" s="3" t="e">
+        <v>3.1950330177630271E-2</v>
+      </c>
+      <c r="K38" s="3">
         <f>B28/Table367[[#This Row],[100 rounds time]] - 1</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+        <v>9.0958281967105092E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E40" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E40" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>8</v>
       </c>
@@ -1420,10 +1603,10 @@
         <v>0</v>
       </c>
       <c r="I41" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>1</v>
       </c>
@@ -1449,7 +1632,7 @@
         <v>4.4264247387365785E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>2</v>
       </c>
@@ -1475,7 +1658,7 @@
         <v>1.27114293729087E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>3</v>
       </c>
@@ -1501,7 +1684,7 @@
         <v>6.16212374344145E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>4</v>
       </c>
@@ -1527,9 +1710,9 @@
         <v>0.33509656872492433</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B46">
         <v>64.991707000000005</v>
@@ -1539,7 +1722,7 @@
         <v>0.6499170700000001</v>
       </c>
       <c r="E46" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F46">
         <v>48.561478000000001</v>
@@ -1553,7 +1736,7 @@
         <v>0.3383387342535169</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>11</v>
       </c>
@@ -1579,25 +1762,438 @@
         <v>2.6989523459723497E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>13</v>
       </c>
+      <c r="B48">
+        <v>570.36041299999999</v>
+      </c>
       <c r="C48">
         <f>Table1012[[#This Row],[100 rounds time]]/100</f>
-        <v>0</v>
+        <v>5.7036041299999996</v>
       </c>
       <c r="E48" t="s">
         <v>13</v>
       </c>
+      <c r="F48">
+        <v>554.48492399999998</v>
+      </c>
       <c r="G48">
         <f>Table10[[#This Row],[100 rounds time]]/100</f>
+        <v>5.5448492399999996</v>
+      </c>
+      <c r="I48" s="3">
+        <f>Table1012[[#This Row],[100 rounds time]]/Table10[[#This Row],[100 rounds time]] - 1</f>
+        <v>2.8631056161952495E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>31</v>
+      </c>
+      <c r="B51" t="s">
+        <v>32</v>
+      </c>
+      <c r="C51" t="s">
+        <v>33</v>
+      </c>
+      <c r="D51" t="s">
+        <v>34</v>
+      </c>
+      <c r="E51" t="s">
+        <v>35</v>
+      </c>
+      <c r="F51" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>1</v>
+      </c>
+      <c r="B52" s="7">
+        <f t="shared" ref="B52:B58" si="0">(100/F11)</f>
+        <v>1317.5924949931484</v>
+      </c>
+      <c r="C52">
+        <f>100/B22</f>
+        <v>1517.957436473481</v>
+      </c>
+      <c r="D52">
+        <f>100/F32</f>
+        <v>2191.4446002805048</v>
+      </c>
+      <c r="E52">
+        <f>100/B42</f>
+        <v>1281.3777373431915</v>
+      </c>
+      <c r="F52">
+        <f>100/F42</f>
+        <v>1338.0969585056134</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>2</v>
+      </c>
+      <c r="B53" s="7">
+        <f t="shared" si="0"/>
+        <v>87.922522673020538</v>
+      </c>
+      <c r="C53">
+        <f t="shared" ref="C53:C58" si="1">100/B23</f>
+        <v>99.425717058271431</v>
+      </c>
+      <c r="D53">
+        <f t="shared" ref="D53:D58" si="2">100/B33</f>
+        <v>145.64542039822371</v>
+      </c>
+      <c r="E53">
+        <f t="shared" ref="E53:E58" si="3">100/B43</f>
+        <v>79.826234253277462</v>
+      </c>
+      <c r="F53">
+        <f t="shared" ref="F53:F58" si="4">100/F43</f>
+        <v>80.84093979209328</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>3</v>
+      </c>
+      <c r="B54" s="7">
+        <f t="shared" si="0"/>
+        <v>21.890950841330536</v>
+      </c>
+      <c r="C54">
+        <f t="shared" si="1"/>
+        <v>24.75281222887935</v>
+      </c>
+      <c r="D54">
+        <f t="shared" si="2"/>
+        <v>46.46991305479267</v>
+      </c>
+      <c r="E54">
+        <f t="shared" si="3"/>
+        <v>24.577512559108918</v>
+      </c>
+      <c r="F54">
+        <f t="shared" si="4"/>
+        <v>26.092009296061072</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>4</v>
+      </c>
+      <c r="B55" s="7">
+        <f t="shared" si="0"/>
+        <v>5.5269437957347698</v>
+      </c>
+      <c r="C55">
+        <f t="shared" si="1"/>
+        <v>6.3452328234071578</v>
+      </c>
+      <c r="D55">
+        <f t="shared" si="2"/>
+        <v>10.209187268040884</v>
+      </c>
+      <c r="E55">
+        <f t="shared" si="3"/>
+        <v>5.7705215905219411</v>
+      </c>
+      <c r="F55">
+        <f t="shared" si="4"/>
+        <v>7.7042035752589362</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>24</v>
+      </c>
+      <c r="B56" s="7">
+        <f t="shared" si="0"/>
+        <v>1.3765062591804365</v>
+      </c>
+      <c r="C56">
+        <f t="shared" si="1"/>
+        <v>1.5947105110846254</v>
+      </c>
+      <c r="D56">
+        <f t="shared" si="2"/>
+        <v>2.5901553427535728</v>
+      </c>
+      <c r="E56">
+        <f t="shared" si="3"/>
+        <v>1.538657847531224</v>
+      </c>
+      <c r="F56">
+        <f t="shared" si="4"/>
+        <v>2.059245396114179</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>11</v>
+      </c>
+      <c r="B57" s="7">
+        <f t="shared" si="0"/>
+        <v>0.34412833641369489</v>
+      </c>
+      <c r="C57">
+        <f t="shared" si="1"/>
+        <v>0.37129544471988007</v>
+      </c>
+      <c r="D57">
+        <f t="shared" si="2"/>
+        <v>0.3800624932196851</v>
+      </c>
+      <c r="E57">
+        <f t="shared" si="3"/>
+        <v>0.28979652348614482</v>
+      </c>
+      <c r="F57">
+        <f t="shared" si="4"/>
+        <v>0.29761799355532043</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>13</v>
+      </c>
+      <c r="B58" s="7">
+        <f t="shared" si="0"/>
+        <v>0.20006540578258925</v>
+      </c>
+      <c r="C58">
+        <f t="shared" si="1"/>
+        <v>0.21022742859418839</v>
+      </c>
+      <c r="D58">
+        <f t="shared" si="2"/>
+        <v>0.22934935432147804</v>
+      </c>
+      <c r="E58">
+        <f t="shared" si="3"/>
+        <v>0.17532773614847635</v>
+      </c>
+      <c r="F58">
+        <f t="shared" si="4"/>
+        <v>0.18034755440889139</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>31</v>
+      </c>
+      <c r="B61" t="s">
+        <v>32</v>
+      </c>
+      <c r="C61" t="s">
+        <v>33</v>
+      </c>
+      <c r="D61" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E61" t="s">
+        <v>35</v>
+      </c>
+      <c r="F61" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>1</v>
+      </c>
+      <c r="B62" s="3">
+        <f t="shared" ref="B62:B68" si="5">B52/B52 - 1</f>
         <v>0</v>
       </c>
-      <c r="I48" s="3" t="e">
-        <f>Table1012[[#This Row],[100 rounds time]]/Table10[[#This Row],[100 rounds time]] - 1</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="C62" s="3">
+        <f t="shared" ref="C62:C68" si="6">C52/B52 - 1</f>
+        <v>0.15206897598591329</v>
+      </c>
+      <c r="D62" s="5">
+        <f t="shared" ref="D62:D68" si="7">D52/B52  - 1</f>
+        <v>0.66321879382889204</v>
+      </c>
+      <c r="E62" s="3">
+        <f t="shared" ref="E62:E68" si="8">E52/B52  - 1</f>
+        <v>-2.7485552466011365E-2</v>
+      </c>
+      <c r="F62" s="3">
+        <f t="shared" ref="F62:F68" si="9">F52/B52  - 1</f>
+        <v>1.5562067627420406E-2</v>
+      </c>
+      <c r="G62" s="3"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>2</v>
+      </c>
+      <c r="B63" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="C63" s="3">
+        <f t="shared" si="6"/>
+        <v>0.13083330681980887</v>
+      </c>
+      <c r="D63" s="6">
+        <f t="shared" si="7"/>
+        <v>0.65652003571225692</v>
+      </c>
+      <c r="E63" s="3">
+        <f t="shared" si="8"/>
+        <v>-9.2084350785210822E-2</v>
+      </c>
+      <c r="F63" s="3">
+        <f t="shared" si="9"/>
+        <v>-8.0543445133658298E-2</v>
+      </c>
+      <c r="G63" s="3"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>3</v>
+      </c>
+      <c r="B64" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="C64" s="3">
+        <f t="shared" si="6"/>
+        <v>0.13073262135994401</v>
+      </c>
+      <c r="D64" s="5">
+        <f t="shared" si="7"/>
+        <v>1.1227909829780707</v>
+      </c>
+      <c r="E64" s="3">
+        <f t="shared" si="8"/>
+        <v>0.122724761352353</v>
+      </c>
+      <c r="F64" s="3">
+        <f t="shared" si="9"/>
+        <v>0.19190845044514271</v>
+      </c>
+      <c r="G64" s="3"/>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>4</v>
+      </c>
+      <c r="B65" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="C65" s="3">
+        <f t="shared" si="6"/>
+        <v>0.14805452306279543</v>
+      </c>
+      <c r="D65" s="6">
+        <f t="shared" si="7"/>
+        <v>0.84716683312746466</v>
+      </c>
+      <c r="E65" s="3">
+        <f t="shared" si="8"/>
+        <v>4.4070973722429407E-2</v>
+      </c>
+      <c r="F65" s="3">
+        <f t="shared" si="9"/>
+        <v>0.39393557452210604</v>
+      </c>
+      <c r="G65" s="3"/>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>24</v>
+      </c>
+      <c r="B66" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="C66" s="3">
+        <f t="shared" si="6"/>
+        <v>0.15852034849017427</v>
+      </c>
+      <c r="D66" s="5">
+        <f t="shared" si="7"/>
+        <v>0.88168802392205303</v>
+      </c>
+      <c r="E66" s="3">
+        <f t="shared" si="8"/>
+        <v>0.11779938323515626</v>
+      </c>
+      <c r="F66" s="3">
+        <f t="shared" si="9"/>
+        <v>0.49599421170830071</v>
+      </c>
+      <c r="G66" s="3"/>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>11</v>
+      </c>
+      <c r="B67" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="C67" s="3">
+        <f t="shared" si="6"/>
+        <v>7.8944700077026475E-2</v>
+      </c>
+      <c r="D67" s="6">
+        <f t="shared" si="7"/>
+        <v>0.10442080178713287</v>
+      </c>
+      <c r="E67" s="3">
+        <f t="shared" si="8"/>
+        <v>-0.15788241530402458</v>
+      </c>
+      <c r="F67" s="3">
+        <f t="shared" si="9"/>
+        <v>-0.13515406299602695</v>
+      </c>
+      <c r="G67" s="3"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>13</v>
+      </c>
+      <c r="B68" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="C68" s="3">
+        <f t="shared" si="6"/>
+        <v>5.079350311388775E-2</v>
+      </c>
+      <c r="D68" s="5">
+        <f t="shared" si="7"/>
+        <v>0.14637187485932279</v>
+      </c>
+      <c r="E68" s="3">
+        <f t="shared" si="8"/>
+        <v>-0.12364791172840384</v>
+      </c>
+      <c r="F68" s="3">
+        <f t="shared" si="9"/>
+        <v>-9.8557025871455317E-2</v>
+      </c>
+      <c r="G68" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1606,7 +2202,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="13">
+  <tableParts count="15">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
@@ -1620,6 +2216,8 @@
     <tablePart r:id="rId12"/>
     <tablePart r:id="rId13"/>
     <tablePart r:id="rId14"/>
+    <tablePart r:id="rId15"/>
+    <tablePart r:id="rId16"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>